<commit_message>
Updates to deal with processing contingencies using line outages
</commit_message>
<xml_diff>
--- a/tests/test_files/Inputs_NoContingencies.xlsx
+++ b/tests/test_files/Inputs_NoContingencies.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90FF45B7-59BD-4F04-A7A2-6E1FCEA1C9DB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D1E56E-F981-4C22-90DC-CC43E21E849D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="868" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33750" yWindow="975" windowWidth="21600" windowHeight="11385" tabRatio="868" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="10" r:id="rId1"/>
     <sheet name="Study_Settings" sheetId="17" r:id="rId2"/>
     <sheet name="Base_Scenarios" sheetId="13" r:id="rId3"/>
-    <sheet name="Contingencies" sheetId="11" r:id="rId4"/>
+    <sheet name="Contingencies_Breakers" sheetId="11" r:id="rId4"/>
     <sheet name="Terminals" sheetId="12" r:id="rId5"/>
     <sheet name="Loadflow_Settings" sheetId="14" r:id="rId6"/>
     <sheet name="Frequency_Sweep" sheetId="15" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Contingencies!$A$5:$AB$166</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Contingencies_Breakers!$A$5:$AB$166</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Terminals!$A$4:$D$103</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -25,7 +25,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -353,7 +355,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="216">
   <si>
     <t>Name</t>
   </si>
@@ -971,9 +973,6 @@
   </si>
   <si>
     <t>375520_LADB_G_1T1</t>
-  </si>
-  <si>
-    <t>Base_Case</t>
   </si>
   <si>
     <t>Include_Intact</t>
@@ -2430,17 +2429,17 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B2" s="46" t="s">
         <v>211</v>
-      </c>
-      <c r="B2" s="46" t="s">
-        <v>212</v>
       </c>
       <c r="C2" s="46"/>
       <c r="D2" s="46"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="47" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B3" s="47"/>
       <c r="C3" s="47"/>
@@ -2476,7 +2475,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B7" s="37" t="s">
         <v>169</v>
@@ -2485,7 +2484,7 @@
         <v>43977</v>
       </c>
       <c r="D7" s="39" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2671,7 +2670,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -2719,7 +2718,7 @@
         <v>170</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -2752,7 +2751,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -2763,7 +2762,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -2790,13 +2789,13 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B12" s="11" t="b">
         <v>1</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -3009,8 +3008,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AB166"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -3205,12 +3204,8 @@
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="B6" s="3">
-        <v>0</v>
-      </c>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>

</xml_diff>